<commit_message>
Edit CV calculation code
</commit_message>
<xml_diff>
--- a/Data/MetaData2.xlsx
+++ b/Data/MetaData2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="544" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="544" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="AdasTables" sheetId="1041" r:id="rId1"/>
@@ -3621,7 +3621,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4806,7 +4806,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5990,8 +5990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="K36" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="R47" sqref="R47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6004,6 +6004,7 @@
     <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="10" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -7167,6 +7168,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -49014,7 +49016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -59690,7 +59692,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G34" sqref="A1:L35"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -72618,7 +72620,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G29" sqref="A1:L35"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -77317,7 +77319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -78495,7 +78497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update CV by using 97 data
</commit_message>
<xml_diff>
--- a/Data/MetaData2.xlsx
+++ b/Data/MetaData2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="544" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="544" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="AdasTables" sheetId="1041" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17277" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17325" uniqueCount="492">
   <si>
     <t>Year</t>
   </si>
@@ -3618,10 +3618,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4796,6 +4796,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="36" spans="1:12">
+      <c r="A36">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
+        <v>299</v>
+      </c>
+      <c r="C36">
+        <v>11117</v>
+      </c>
+      <c r="D36">
+        <v>11117</v>
+      </c>
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" t="s">
+        <v>277</v>
+      </c>
+      <c r="I36" t="s">
+        <v>68</v>
+      </c>
+      <c r="J36" t="s">
+        <v>69</v>
+      </c>
+      <c r="K36" t="s">
+        <v>70</v>
+      </c>
+      <c r="L36" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4803,10 +4838,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5981,6 +6016,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="36" spans="1:12">
+      <c r="A36">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
+        <v>299</v>
+      </c>
+      <c r="C36">
+        <v>11531</v>
+      </c>
+      <c r="D36">
+        <v>11531</v>
+      </c>
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" t="s">
+        <v>277</v>
+      </c>
+      <c r="I36" t="s">
+        <v>68</v>
+      </c>
+      <c r="J36" t="s">
+        <v>69</v>
+      </c>
+      <c r="K36" t="s">
+        <v>70</v>
+      </c>
+      <c r="L36" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5988,10 +6058,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K36" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="R47" sqref="R47"/>
+    <sheetView topLeftCell="A27" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7163,6 +7233,41 @@
         <v>70</v>
       </c>
       <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
+        <v>299</v>
+      </c>
+      <c r="C36">
+        <v>11231</v>
+      </c>
+      <c r="D36">
+        <v>11231</v>
+      </c>
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" t="s">
+        <v>277</v>
+      </c>
+      <c r="I36" t="s">
+        <v>68</v>
+      </c>
+      <c r="J36" t="s">
+        <v>69</v>
+      </c>
+      <c r="K36" t="s">
+        <v>70</v>
+      </c>
+      <c r="L36" t="s">
         <v>72</v>
       </c>
     </row>
@@ -59689,10 +59794,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -60864,6 +60969,41 @@
         <v>70</v>
       </c>
       <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
+        <v>299</v>
+      </c>
+      <c r="C36">
+        <v>11441</v>
+      </c>
+      <c r="D36">
+        <v>11441</v>
+      </c>
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" t="s">
+        <v>277</v>
+      </c>
+      <c r="I36" t="s">
+        <v>68</v>
+      </c>
+      <c r="J36" t="s">
+        <v>69</v>
+      </c>
+      <c r="K36" t="s">
+        <v>70</v>
+      </c>
+      <c r="L36" t="s">
         <v>72</v>
       </c>
     </row>
@@ -72617,10 +72757,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -73785,6 +73925,41 @@
         <v>70</v>
       </c>
       <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
+        <v>299</v>
+      </c>
+      <c r="C36">
+        <v>11811</v>
+      </c>
+      <c r="D36">
+        <v>11811</v>
+      </c>
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" t="s">
+        <v>277</v>
+      </c>
+      <c r="I36" t="s">
+        <v>68</v>
+      </c>
+      <c r="J36" t="s">
+        <v>69</v>
+      </c>
+      <c r="K36" t="s">
+        <v>70</v>
+      </c>
+      <c r="L36" t="s">
         <v>72</v>
       </c>
     </row>
@@ -77317,10 +77492,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -78485,6 +78660,41 @@
         <v>70</v>
       </c>
       <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
+        <v>299</v>
+      </c>
+      <c r="C36">
+        <v>11812</v>
+      </c>
+      <c r="D36">
+        <v>11812</v>
+      </c>
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" t="s">
+        <v>277</v>
+      </c>
+      <c r="I36" t="s">
+        <v>68</v>
+      </c>
+      <c r="J36" t="s">
+        <v>69</v>
+      </c>
+      <c r="K36" t="s">
+        <v>70</v>
+      </c>
+      <c r="L36" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>